<commit_message>
raw data + loader
</commit_message>
<xml_diff>
--- a/data/RAW/Human_labelling_violentMovie.xlsx
+++ b/data/RAW/Human_labelling_violentMovie.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djay/Desktop/ADA/ada-2024-project-alligatorsdontapologize24/data/RAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD044C8-86D9-C14E-9C21-4807201C5C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A61CFD-BD49-944F-81BE-D723549B8754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="760" windowWidth="15860" windowHeight="17440" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
+    <workbookView xWindow="10840" yWindow="760" windowWidth="15860" windowHeight="17440" activeTab="1" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="label" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -471,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B92C561-11BB-6946-9D59-BAB10DC0BC04}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1263,6 +1263,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1281,16 +1291,6 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1298,7 +1298,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{288373DC-AB41-7043-A0D5-A904531DB146}">
           <x14:formula1>
-            <xm:f>Sheet2!$B$2:$B$4</xm:f>
+            <xm:f>label!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B49 B51:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -1312,7 +1312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE620F0E-B7D1-CC40-BEDA-A8FB3E9B14F4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
last update on the llm
</commit_message>
<xml_diff>
--- a/data/RAW/Human_labelling_violentMovie.xlsx
+++ b/data/RAW/Human_labelling_violentMovie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djay/Desktop/ADA/ada-2024-project-alligatorsdontapologize24/data/RAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4600FB9-10DC-9F42-BA39-4776393B26D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4220AA5C-3504-DD4E-82BB-A481BD9830DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-920" yWindow="760" windowWidth="17280" windowHeight="17440" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15740" windowHeight="17440" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -48,12 +48,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Medium/not sure</t>
-  </si>
-  <si>
     <t>Violent</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>Wikipedia movie ID</t>
+  </si>
+  <si>
+    <t>Peaceful</t>
+  </si>
+  <si>
+    <t>Mild</t>
   </si>
 </sst>
 </file>
@@ -127,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -136,6 +136,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B92C561-11BB-6946-9D59-BAB10DC0BC04}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:F221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,18 +488,18 @@
     <col min="1" max="3" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>19286405</v>
       </c>
@@ -503,8 +509,11 @@
       <c r="C2">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>6714641</v>
       </c>
@@ -514,8 +523,11 @@
       <c r="C3">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>27573594</v>
       </c>
@@ -525,8 +537,11 @@
       <c r="C4">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>25874731</v>
       </c>
@@ -536,8 +551,11 @@
       <c r="C5">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>34954266</v>
       </c>
@@ -547,8 +565,11 @@
       <c r="C6">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>19795169</v>
       </c>
@@ -558,8 +579,11 @@
       <c r="C7">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>21787356</v>
       </c>
@@ -569,8 +593,11 @@
       <c r="C8">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>29651684</v>
       </c>
@@ -580,8 +607,11 @@
       <c r="C9">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>26015405</v>
       </c>
@@ -591,8 +621,11 @@
       <c r="C10">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>16994537</v>
       </c>
@@ -602,8 +635,11 @@
       <c r="C11">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>26363490</v>
       </c>
@@ -613,8 +649,11 @@
       <c r="C12">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>31419116</v>
       </c>
@@ -624,8 +663,11 @@
       <c r="C13">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>9612611</v>
       </c>
@@ -635,8 +677,11 @@
       <c r="C14">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>20176769</v>
       </c>
@@ -646,8 +691,11 @@
       <c r="C15">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>26340503</v>
       </c>
@@ -657,8 +705,11 @@
       <c r="C16">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>33440196</v>
       </c>
@@ -668,8 +719,11 @@
       <c r="C17">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>19069841</v>
       </c>
@@ -679,8 +733,11 @@
       <c r="C18">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>34985277</v>
       </c>
@@ -690,8 +747,11 @@
       <c r="C19">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>4481850</v>
       </c>
@@ -701,8 +761,11 @@
       <c r="C20">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>24328926</v>
       </c>
@@ -712,8 +775,11 @@
       <c r="C21">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>6493287</v>
       </c>
@@ -723,8 +789,11 @@
       <c r="C22">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>15323823</v>
       </c>
@@ -734,8 +803,11 @@
       <c r="C23">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>30465048</v>
       </c>
@@ -745,8 +817,11 @@
       <c r="C24">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>34430499</v>
       </c>
@@ -756,8 +831,11 @@
       <c r="C25">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>18050522</v>
       </c>
@@ -767,8 +845,11 @@
       <c r="C26">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>28852030</v>
       </c>
@@ -778,8 +859,11 @@
       <c r="C27">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>2967223</v>
       </c>
@@ -789,8 +873,11 @@
       <c r="C28">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>27606335</v>
       </c>
@@ -800,8 +887,11 @@
       <c r="C29">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>24398624</v>
       </c>
@@ -811,8 +901,11 @@
       <c r="C30">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>15124157</v>
       </c>
@@ -822,8 +915,11 @@
       <c r="C31">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>6493287</v>
       </c>
@@ -833,8 +929,11 @@
       <c r="C32">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>15323823</v>
       </c>
@@ -844,8 +943,11 @@
       <c r="C33">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>30465048</v>
       </c>
@@ -855,8 +957,11 @@
       <c r="C34">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34430499</v>
       </c>
@@ -866,8 +971,11 @@
       <c r="C35">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>18050522</v>
       </c>
@@ -877,8 +985,11 @@
       <c r="C36">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>28852030</v>
       </c>
@@ -888,8 +999,11 @@
       <c r="C37">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>2967223</v>
       </c>
@@ -899,8 +1013,11 @@
       <c r="C38">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>27606335</v>
       </c>
@@ -910,8 +1027,11 @@
       <c r="C39">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>24398624</v>
       </c>
@@ -921,8 +1041,11 @@
       <c r="C40">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>15124157</v>
       </c>
@@ -932,8 +1055,11 @@
       <c r="C41">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>8555713</v>
       </c>
@@ -943,8 +1069,11 @@
       <c r="C42">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>22620682</v>
       </c>
@@ -954,8 +1083,11 @@
       <c r="C43">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>32109549</v>
       </c>
@@ -965,8 +1097,11 @@
       <c r="C44">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>26708843</v>
       </c>
@@ -976,8 +1111,11 @@
       <c r="C45">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>29584842</v>
       </c>
@@ -987,8 +1125,11 @@
       <c r="C46">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>36039685</v>
       </c>
@@ -998,8 +1139,11 @@
       <c r="C47">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>16494542</v>
       </c>
@@ -1009,8 +1153,11 @@
       <c r="C48">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>34358984</v>
       </c>
@@ -1020,8 +1167,11 @@
       <c r="C49">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>24165847</v>
       </c>
@@ -1031,8 +1181,11 @@
       <c r="C50">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>5766332</v>
       </c>
@@ -1042,8 +1195,11 @@
       <c r="C51">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>14060163</v>
       </c>
@@ -1053,8 +1209,11 @@
       <c r="C52">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>113454</v>
       </c>
@@ -1064,8 +1223,11 @@
       <c r="C53">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>15217227</v>
       </c>
@@ -1075,8 +1237,11 @@
       <c r="C54">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>28807164</v>
       </c>
@@ -1086,8 +1251,11 @@
       <c r="C55">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>27286055</v>
       </c>
@@ -1097,8 +1265,11 @@
       <c r="C56">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>24104622</v>
       </c>
@@ -1108,8 +1279,11 @@
       <c r="C57">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>14144257</v>
       </c>
@@ -1119,8 +1293,11 @@
       <c r="C58">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>35004480</v>
       </c>
@@ -1130,8 +1307,11 @@
       <c r="C59">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>3868321</v>
       </c>
@@ -1141,8 +1321,11 @@
       <c r="C60">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>2295249</v>
       </c>
@@ -1152,8 +1335,11 @@
       <c r="C61">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>14060163</v>
       </c>
@@ -1163,8 +1349,11 @@
       <c r="C62">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>113454</v>
       </c>
@@ -1174,8 +1363,11 @@
       <c r="C63">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>15217227</v>
       </c>
@@ -1185,8 +1377,11 @@
       <c r="C64">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>28807164</v>
       </c>
@@ -1196,8 +1391,11 @@
       <c r="C65">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>27286055</v>
       </c>
@@ -1207,8 +1405,11 @@
       <c r="C66">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>24104622</v>
       </c>
@@ -1218,8 +1419,11 @@
       <c r="C67">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>14144257</v>
       </c>
@@ -1229,8 +1433,11 @@
       <c r="C68">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>35004480</v>
       </c>
@@ -1240,8 +1447,11 @@
       <c r="C69">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>3868321</v>
       </c>
@@ -1251,8 +1461,11 @@
       <c r="C70">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>2295249</v>
       </c>
@@ -1262,8 +1475,11 @@
       <c r="C71">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>14060163</v>
       </c>
@@ -1273,8 +1489,11 @@
       <c r="C72">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>113454</v>
       </c>
@@ -1284,8 +1503,11 @@
       <c r="C73">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>15217227</v>
       </c>
@@ -1295,8 +1517,11 @@
       <c r="C74">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>28807164</v>
       </c>
@@ -1306,8 +1531,11 @@
       <c r="C75">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>27286055</v>
       </c>
@@ -1317,8 +1545,11 @@
       <c r="C76">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>24104622</v>
       </c>
@@ -1328,8 +1559,11 @@
       <c r="C77">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>14144257</v>
       </c>
@@ -1339,8 +1573,11 @@
       <c r="C78">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>35004480</v>
       </c>
@@ -1350,8 +1587,11 @@
       <c r="C79">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>3868321</v>
       </c>
@@ -1361,8 +1601,11 @@
       <c r="C80">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>2295249</v>
       </c>
@@ -1372,8 +1615,11 @@
       <c r="C81">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>19286405</v>
       </c>
@@ -1383,8 +1629,11 @@
       <c r="C82">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>6714641</v>
       </c>
@@ -1394,8 +1643,11 @@
       <c r="C83">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>27573594</v>
       </c>
@@ -1405,8 +1657,11 @@
       <c r="C84">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>25874731</v>
       </c>
@@ -1416,8 +1671,11 @@
       <c r="C85">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>34954266</v>
       </c>
@@ -1427,8 +1685,11 @@
       <c r="C86">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>19795169</v>
       </c>
@@ -1438,8 +1699,11 @@
       <c r="C87">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>21787356</v>
       </c>
@@ -1449,8 +1713,11 @@
       <c r="C88">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>29651684</v>
       </c>
@@ -1460,8 +1727,11 @@
       <c r="C89">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>26015405</v>
       </c>
@@ -1471,8 +1741,11 @@
       <c r="C90">
         <v>13.11</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>16994537</v>
       </c>
@@ -1482,10 +1755,1873 @@
       <c r="C91">
         <v>13.11</v>
       </c>
+      <c r="D91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>3477618</v>
+      </c>
+      <c r="B92">
+        <v>-1</v>
+      </c>
+      <c r="C92">
+        <v>14.11</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
+        <v>18950355</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>14.11</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>35784403</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>14.11</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="5">
+        <v>29133141</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>14.11</v>
+      </c>
+      <c r="D95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
+        <v>8411320</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>14.11</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="5">
+        <v>19389678</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>14.11</v>
+      </c>
+      <c r="D97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
+        <v>23283544</v>
+      </c>
+      <c r="B98">
+        <v>-1</v>
+      </c>
+      <c r="C98">
+        <v>14.11</v>
+      </c>
+      <c r="D98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="5">
+        <v>24631652</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>14.11</v>
+      </c>
+      <c r="D99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="5">
+        <v>28074095</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>14.11</v>
+      </c>
+      <c r="D100">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="5">
+        <v>24815671</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>14.11</v>
+      </c>
+      <c r="D101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="5">
+        <v>3477618</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>14.11</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="5">
+        <v>18950355</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>14.11</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="5">
+        <v>35784403</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>14.11</v>
+      </c>
+      <c r="D104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="5">
+        <v>29133141</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>14.11</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="5">
+        <v>8411320</v>
+      </c>
+      <c r="B106">
+        <v>-1</v>
+      </c>
+      <c r="C106">
+        <v>14.11</v>
+      </c>
+      <c r="D106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="5">
+        <v>19389678</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>14.11</v>
+      </c>
+      <c r="D107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="5">
+        <v>23283544</v>
+      </c>
+      <c r="B108">
+        <v>-1</v>
+      </c>
+      <c r="C108">
+        <v>14.11</v>
+      </c>
+      <c r="D108">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="5">
+        <v>24631652</v>
+      </c>
+      <c r="B109">
+        <v>-1</v>
+      </c>
+      <c r="C109">
+        <v>14.11</v>
+      </c>
+      <c r="D109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="5">
+        <v>28074095</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>14.11</v>
+      </c>
+      <c r="D110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="5">
+        <v>24815671</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>14.11</v>
+      </c>
+      <c r="D111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
+        <v>3477618</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>14.11</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="5">
+        <v>18950355</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>14.11</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="5">
+        <v>35784403</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>14.11</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="5">
+        <v>29133141</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>14.11</v>
+      </c>
+      <c r="D115">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="5">
+        <v>8411320</v>
+      </c>
+      <c r="B116">
+        <v>-1</v>
+      </c>
+      <c r="C116">
+        <v>14.11</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="5">
+        <v>19389678</v>
+      </c>
+      <c r="B117">
+        <v>-1</v>
+      </c>
+      <c r="C117">
+        <v>14.11</v>
+      </c>
+      <c r="D117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="5">
+        <v>23283544</v>
+      </c>
+      <c r="B118">
+        <v>-1</v>
+      </c>
+      <c r="C118">
+        <v>14.11</v>
+      </c>
+      <c r="D118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="5">
+        <v>24631652</v>
+      </c>
+      <c r="B119">
+        <v>-1</v>
+      </c>
+      <c r="C119">
+        <v>14.11</v>
+      </c>
+      <c r="D119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
+        <v>28074095</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>14.11</v>
+      </c>
+      <c r="D120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="5">
+        <v>24815671</v>
+      </c>
+      <c r="B121">
+        <v>-1</v>
+      </c>
+      <c r="C121">
+        <v>14.11</v>
+      </c>
+      <c r="D121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="6">
+        <v>25960460</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>14.11</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="6">
+        <v>32104837</v>
+      </c>
+      <c r="B123">
+        <v>-1</v>
+      </c>
+      <c r="C123">
+        <v>14.11</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>7028314</v>
+      </c>
+      <c r="B124">
+        <v>-1</v>
+      </c>
+      <c r="C124">
+        <v>14.11</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>12788657</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <v>14.11</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="6">
+        <v>2154704</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>14.11</v>
+      </c>
+      <c r="D126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>33872851</v>
+      </c>
+      <c r="B127">
+        <v>-1</v>
+      </c>
+      <c r="C127">
+        <v>14.11</v>
+      </c>
+      <c r="D127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="6">
+        <v>16304395</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>14.11</v>
+      </c>
+      <c r="D128">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>30109815</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>14.11</v>
+      </c>
+      <c r="D129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="6">
+        <v>37067980</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>14.11</v>
+      </c>
+      <c r="D130">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>25947106</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>14.11</v>
+      </c>
+      <c r="D131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>14881706</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>14.11</v>
+      </c>
+      <c r="D132">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>3883051</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>14.11</v>
+      </c>
+      <c r="D133">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="6">
+        <v>21236198</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>14.11</v>
+      </c>
+      <c r="D134">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>17594419</v>
+      </c>
+      <c r="B135">
+        <v>-1</v>
+      </c>
+      <c r="C135">
+        <v>14.11</v>
+      </c>
+      <c r="D135">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="6">
+        <v>5254729</v>
+      </c>
+      <c r="B136">
+        <v>-1</v>
+      </c>
+      <c r="C136">
+        <v>14.11</v>
+      </c>
+      <c r="D136">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>24291753</v>
+      </c>
+      <c r="B137">
+        <v>-1</v>
+      </c>
+      <c r="C137">
+        <v>14.11</v>
+      </c>
+      <c r="D137">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="6">
+        <v>11686007</v>
+      </c>
+      <c r="B138">
+        <v>-1</v>
+      </c>
+      <c r="C138">
+        <v>14.11</v>
+      </c>
+      <c r="D138">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="6">
+        <v>9086301</v>
+      </c>
+      <c r="B139">
+        <v>-1</v>
+      </c>
+      <c r="C139">
+        <v>14.11</v>
+      </c>
+      <c r="D139">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="6">
+        <v>29499560</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>14.11</v>
+      </c>
+      <c r="D140">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="6">
+        <v>7985961</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>14.11</v>
+      </c>
+      <c r="D141">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="6">
+        <v>25960460</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>14.11</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="6">
+        <v>32104837</v>
+      </c>
+      <c r="B143">
+        <v>-1</v>
+      </c>
+      <c r="C143">
+        <v>14.11</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="6">
+        <v>7028314</v>
+      </c>
+      <c r="B144">
+        <v>-1</v>
+      </c>
+      <c r="C144">
+        <v>14.11</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="6">
+        <v>12788657</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>14.11</v>
+      </c>
+      <c r="D145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="6">
+        <v>2154704</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>14.11</v>
+      </c>
+      <c r="D146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="6">
+        <v>33872851</v>
+      </c>
+      <c r="B147">
+        <v>-1</v>
+      </c>
+      <c r="C147">
+        <v>14.11</v>
+      </c>
+      <c r="D147">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="6">
+        <v>16304395</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>14.11</v>
+      </c>
+      <c r="D148">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="6">
+        <v>30109815</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>14.11</v>
+      </c>
+      <c r="D149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="6">
+        <v>37067980</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>14.11</v>
+      </c>
+      <c r="D150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="6">
+        <v>25947106</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>14.11</v>
+      </c>
+      <c r="D151">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="6">
+        <v>14881706</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>14.11</v>
+      </c>
+      <c r="D152">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="6">
+        <v>3883051</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>14.11</v>
+      </c>
+      <c r="D153">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="6">
+        <v>21236198</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>14.11</v>
+      </c>
+      <c r="D154">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="6">
+        <v>17594419</v>
+      </c>
+      <c r="B155">
+        <v>-1</v>
+      </c>
+      <c r="C155">
+        <v>14.11</v>
+      </c>
+      <c r="D155">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="6">
+        <v>5254729</v>
+      </c>
+      <c r="B156">
+        <v>-1</v>
+      </c>
+      <c r="C156">
+        <v>14.11</v>
+      </c>
+      <c r="D156">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="6">
+        <v>24291753</v>
+      </c>
+      <c r="B157">
+        <v>-1</v>
+      </c>
+      <c r="C157">
+        <v>14.11</v>
+      </c>
+      <c r="D157">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="6">
+        <v>11686007</v>
+      </c>
+      <c r="B158">
+        <v>-1</v>
+      </c>
+      <c r="C158">
+        <v>14.11</v>
+      </c>
+      <c r="D158">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="6">
+        <v>9086301</v>
+      </c>
+      <c r="B159">
+        <v>-1</v>
+      </c>
+      <c r="C159">
+        <v>14.11</v>
+      </c>
+      <c r="D159">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="6">
+        <v>29499560</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>14.11</v>
+      </c>
+      <c r="D160">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="6">
+        <v>7985961</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>14.11</v>
+      </c>
+      <c r="D161">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="6">
+        <v>18890079</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>14.11</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="6">
+        <v>22657183</v>
+      </c>
+      <c r="B163">
+        <v>-1</v>
+      </c>
+      <c r="C163">
+        <v>14.11</v>
+      </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="6">
+        <v>12746610</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>14.11</v>
+      </c>
+      <c r="D164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="6">
+        <v>31839719</v>
+      </c>
+      <c r="B165">
+        <v>-1</v>
+      </c>
+      <c r="C165">
+        <v>14.11</v>
+      </c>
+      <c r="D165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="6">
+        <v>13292846</v>
+      </c>
+      <c r="B166">
+        <v>-1</v>
+      </c>
+      <c r="C166">
+        <v>14.11</v>
+      </c>
+      <c r="D166">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="6">
+        <v>17352897</v>
+      </c>
+      <c r="B167">
+        <v>-1</v>
+      </c>
+      <c r="C167">
+        <v>14.11</v>
+      </c>
+      <c r="D167">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="6">
+        <v>21472296</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>14.11</v>
+      </c>
+      <c r="D168">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="6">
+        <v>34383684</v>
+      </c>
+      <c r="B169">
+        <v>-1</v>
+      </c>
+      <c r="C169">
+        <v>14.11</v>
+      </c>
+      <c r="D169">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="6">
+        <v>27286055</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>14.11</v>
+      </c>
+      <c r="D170">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="6">
+        <v>20981095</v>
+      </c>
+      <c r="B171">
+        <v>-1</v>
+      </c>
+      <c r="C171">
+        <v>14.11</v>
+      </c>
+      <c r="D171">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="6">
+        <v>16494542</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>14.11</v>
+      </c>
+      <c r="D172">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="6">
+        <v>15354287</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>14.11</v>
+      </c>
+      <c r="D173">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="6">
+        <v>4180145</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>14.11</v>
+      </c>
+      <c r="D174">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="6">
+        <v>28932258</v>
+      </c>
+      <c r="B175">
+        <v>-1</v>
+      </c>
+      <c r="C175">
+        <v>14.11</v>
+      </c>
+      <c r="D175">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="6">
+        <v>26016562</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>14.11</v>
+      </c>
+      <c r="D176">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="6">
+        <v>909664</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
+      </c>
+      <c r="C177">
+        <v>14.11</v>
+      </c>
+      <c r="D177">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="6">
+        <v>3597370</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>14.11</v>
+      </c>
+      <c r="D178">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="6">
+        <v>29449916</v>
+      </c>
+      <c r="B179">
+        <v>-1</v>
+      </c>
+      <c r="C179">
+        <v>14.11</v>
+      </c>
+      <c r="D179">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="6">
+        <v>25183068</v>
+      </c>
+      <c r="B180">
+        <v>-1</v>
+      </c>
+      <c r="C180">
+        <v>14.11</v>
+      </c>
+      <c r="D180">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="6">
+        <v>14336079</v>
+      </c>
+      <c r="B181">
+        <v>-1</v>
+      </c>
+      <c r="C181">
+        <v>14.11</v>
+      </c>
+      <c r="D181">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="6">
+        <v>18890079</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>14.11</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="F182" s="6"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="6">
+        <v>22657183</v>
+      </c>
+      <c r="B183">
+        <v>-1</v>
+      </c>
+      <c r="C183">
+        <v>14.11</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+      <c r="F183" s="6"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="6">
+        <v>12746610</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>14.11</v>
+      </c>
+      <c r="D184">
+        <v>3</v>
+      </c>
+      <c r="F184" s="6"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="6">
+        <v>31839719</v>
+      </c>
+      <c r="B185">
+        <v>-1</v>
+      </c>
+      <c r="C185">
+        <v>14.11</v>
+      </c>
+      <c r="D185">
+        <v>4</v>
+      </c>
+      <c r="F185" s="6"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="6">
+        <v>13292846</v>
+      </c>
+      <c r="B186">
+        <v>-1</v>
+      </c>
+      <c r="C186">
+        <v>14.11</v>
+      </c>
+      <c r="D186">
+        <v>5</v>
+      </c>
+      <c r="F186" s="6"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="6">
+        <v>17352897</v>
+      </c>
+      <c r="B187">
+        <v>-1</v>
+      </c>
+      <c r="C187">
+        <v>14.11</v>
+      </c>
+      <c r="D187">
+        <v>6</v>
+      </c>
+      <c r="F187" s="6"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="6">
+        <v>21472296</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>14.11</v>
+      </c>
+      <c r="D188">
+        <v>7</v>
+      </c>
+      <c r="F188" s="6"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="6">
+        <v>34383684</v>
+      </c>
+      <c r="B189">
+        <v>-1</v>
+      </c>
+      <c r="C189">
+        <v>14.11</v>
+      </c>
+      <c r="D189">
+        <v>8</v>
+      </c>
+      <c r="F189" s="6"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="6">
+        <v>27286055</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+      <c r="C190">
+        <v>14.11</v>
+      </c>
+      <c r="D190">
+        <v>9</v>
+      </c>
+      <c r="F190" s="6"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="6">
+        <v>20981095</v>
+      </c>
+      <c r="B191">
+        <v>-1</v>
+      </c>
+      <c r="C191">
+        <v>14.11</v>
+      </c>
+      <c r="D191">
+        <v>10</v>
+      </c>
+      <c r="F191" s="6"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="6">
+        <v>16494542</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192">
+        <v>14.11</v>
+      </c>
+      <c r="D192">
+        <v>11</v>
+      </c>
+      <c r="F192" s="6"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="6">
+        <v>15354287</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>14.11</v>
+      </c>
+      <c r="D193">
+        <v>12</v>
+      </c>
+      <c r="F193" s="6"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="6">
+        <v>4180145</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>14.11</v>
+      </c>
+      <c r="D194">
+        <v>13</v>
+      </c>
+      <c r="F194" s="6"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="6">
+        <v>28932258</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>14.11</v>
+      </c>
+      <c r="D195">
+        <v>14</v>
+      </c>
+      <c r="F195" s="6"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="6">
+        <v>26016562</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <v>14.11</v>
+      </c>
+      <c r="D196">
+        <v>15</v>
+      </c>
+      <c r="F196" s="6"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="6">
+        <v>909664</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="C197">
+        <v>14.11</v>
+      </c>
+      <c r="D197">
+        <v>16</v>
+      </c>
+      <c r="F197" s="6"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="6">
+        <v>3597370</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>14.11</v>
+      </c>
+      <c r="D198">
+        <v>17</v>
+      </c>
+      <c r="F198" s="6"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="6">
+        <v>29449916</v>
+      </c>
+      <c r="B199">
+        <v>-1</v>
+      </c>
+      <c r="C199">
+        <v>14.11</v>
+      </c>
+      <c r="D199">
+        <v>18</v>
+      </c>
+      <c r="F199" s="6"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" s="6">
+        <v>25183068</v>
+      </c>
+      <c r="B200">
+        <v>-1</v>
+      </c>
+      <c r="C200">
+        <v>14.11</v>
+      </c>
+      <c r="D200">
+        <v>19</v>
+      </c>
+      <c r="F200" s="6"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" s="6">
+        <v>14336079</v>
+      </c>
+      <c r="B201">
+        <v>-1</v>
+      </c>
+      <c r="C201">
+        <v>14.11</v>
+      </c>
+      <c r="D201">
+        <v>20</v>
+      </c>
+      <c r="F201" s="6"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="6">
+        <v>18890079</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <v>14.11</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+      <c r="F202" s="6"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="6">
+        <v>22657183</v>
+      </c>
+      <c r="B203">
+        <v>-1</v>
+      </c>
+      <c r="C203">
+        <v>14.11</v>
+      </c>
+      <c r="D203">
+        <v>2</v>
+      </c>
+      <c r="F203" s="6"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="6">
+        <v>12746610</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>14.11</v>
+      </c>
+      <c r="D204">
+        <v>3</v>
+      </c>
+      <c r="F204" s="6"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" s="6">
+        <v>31839719</v>
+      </c>
+      <c r="B205">
+        <v>-1</v>
+      </c>
+      <c r="C205">
+        <v>14.11</v>
+      </c>
+      <c r="D205">
+        <v>4</v>
+      </c>
+      <c r="F205" s="6"/>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" s="6">
+        <v>13292846</v>
+      </c>
+      <c r="B206">
+        <v>-1</v>
+      </c>
+      <c r="C206">
+        <v>14.11</v>
+      </c>
+      <c r="D206">
+        <v>5</v>
+      </c>
+      <c r="F206" s="6"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="6">
+        <v>17352897</v>
+      </c>
+      <c r="B207">
+        <v>-1</v>
+      </c>
+      <c r="C207">
+        <v>14.11</v>
+      </c>
+      <c r="D207">
+        <v>6</v>
+      </c>
+      <c r="F207" s="6"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="6">
+        <v>21472296</v>
+      </c>
+      <c r="B208">
+        <v>-1</v>
+      </c>
+      <c r="C208">
+        <v>14.11</v>
+      </c>
+      <c r="D208">
+        <v>7</v>
+      </c>
+      <c r="F208" s="6"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="6">
+        <v>34383684</v>
+      </c>
+      <c r="B209">
+        <v>-1</v>
+      </c>
+      <c r="C209">
+        <v>14.11</v>
+      </c>
+      <c r="D209">
+        <v>8</v>
+      </c>
+      <c r="F209" s="6"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="6">
+        <v>27286055</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+      <c r="C210">
+        <v>14.11</v>
+      </c>
+      <c r="D210">
+        <v>9</v>
+      </c>
+      <c r="F210" s="6"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="6">
+        <v>20981095</v>
+      </c>
+      <c r="B211">
+        <v>-1</v>
+      </c>
+      <c r="C211">
+        <v>14.11</v>
+      </c>
+      <c r="D211">
+        <v>10</v>
+      </c>
+      <c r="F211" s="6"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="6">
+        <v>16494542</v>
+      </c>
+      <c r="B212">
+        <v>1</v>
+      </c>
+      <c r="C212">
+        <v>14.11</v>
+      </c>
+      <c r="D212">
+        <v>11</v>
+      </c>
+      <c r="F212" s="6"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="6">
+        <v>15354287</v>
+      </c>
+      <c r="B213">
+        <v>1</v>
+      </c>
+      <c r="C213">
+        <v>14.11</v>
+      </c>
+      <c r="D213">
+        <v>12</v>
+      </c>
+      <c r="F213" s="6"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="6">
+        <v>4180145</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+      <c r="C214">
+        <v>14.11</v>
+      </c>
+      <c r="D214">
+        <v>13</v>
+      </c>
+      <c r="F214" s="6"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="6">
+        <v>28932258</v>
+      </c>
+      <c r="B215">
+        <v>-1</v>
+      </c>
+      <c r="C215">
+        <v>14.11</v>
+      </c>
+      <c r="D215">
+        <v>14</v>
+      </c>
+      <c r="F215" s="6"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" s="6">
+        <v>26016562</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>14.11</v>
+      </c>
+      <c r="D216">
+        <v>15</v>
+      </c>
+      <c r="F216" s="6"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="6">
+        <v>909664</v>
+      </c>
+      <c r="B217">
+        <v>1</v>
+      </c>
+      <c r="C217">
+        <v>14.11</v>
+      </c>
+      <c r="D217">
+        <v>16</v>
+      </c>
+      <c r="F217" s="6"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="6">
+        <v>3597370</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>14.11</v>
+      </c>
+      <c r="D218">
+        <v>17</v>
+      </c>
+      <c r="F218" s="6"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="6">
+        <v>29449916</v>
+      </c>
+      <c r="B219">
+        <v>-1</v>
+      </c>
+      <c r="C219">
+        <v>14.11</v>
+      </c>
+      <c r="D219">
+        <v>18</v>
+      </c>
+      <c r="F219" s="6"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="6">
+        <v>25183068</v>
+      </c>
+      <c r="B220">
+        <v>-1</v>
+      </c>
+      <c r="C220">
+        <v>14.11</v>
+      </c>
+      <c r="D220">
+        <v>19</v>
+      </c>
+      <c r="F220" s="6"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="6">
+        <v>14336079</v>
+      </c>
+      <c r="B221">
+        <v>-1</v>
+      </c>
+      <c r="C221">
+        <v>14.11</v>
+      </c>
+      <c r="D221">
+        <v>20</v>
+      </c>
+      <c r="F221" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B1:B103 B222:B1048576">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1495,7 +3631,7 @@
         <color theme="6" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1505,12 +3641,302 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95:E103">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94:B121 B222:B229">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B121 B222:B1048576">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G182:G222">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G182:G222">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G182:G222">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122:B161">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122:B161">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122:B161">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B164:B181">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B162:B181">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B162:B181">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B182:B221">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B182:B221">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1523,7 +3949,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,7 +3967,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>-1</v>
@@ -1549,7 +3975,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -1557,7 +3983,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
human labelling step is done
</commit_message>
<xml_diff>
--- a/data/RAW/Human_labelling_violentMovie.xlsx
+++ b/data/RAW/Human_labelling_violentMovie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djay/Desktop/ADA/ada-2024-project-alligatorsdontapologize24/data/RAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4220AA5C-3504-DD4E-82BB-A481BD9830DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E9EC7-370F-F84C-8242-F37883193F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15740" windowHeight="17440" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Answer</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Mild</t>
+  </si>
+  <si>
+    <t>LAST</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -141,6 +144,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B92C561-11BB-6946-9D59-BAB10DC0BC04}">
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="B299" sqref="B299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,6 +504,9 @@
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
@@ -510,7 +519,7 @@
         <v>11.11</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,7 +533,7 @@
         <v>11.11</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -538,7 +547,7 @@
         <v>11.11</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,7 +561,7 @@
         <v>11.11</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,7 +575,7 @@
         <v>11.11</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -580,7 +589,7 @@
         <v>11.11</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -594,7 +603,7 @@
         <v>11.11</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -608,7 +617,7 @@
         <v>11.11</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -622,7 +631,7 @@
         <v>11.11</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -636,7 +645,7 @@
         <v>11.11</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -650,7 +659,7 @@
         <v>11.11</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -664,7 +673,7 @@
         <v>11.11</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +687,7 @@
         <v>11.11</v>
       </c>
       <c r="D14">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -692,7 +701,7 @@
         <v>11.11</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,7 +715,7 @@
         <v>11.11</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,7 +729,7 @@
         <v>11.11</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -734,7 +743,7 @@
         <v>11.11</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,7 +757,7 @@
         <v>11.11</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -762,7 +771,7 @@
         <v>11.11</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,7 +785,7 @@
         <v>11.11</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -790,7 +799,7 @@
         <v>11.11</v>
       </c>
       <c r="D22">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -804,7 +813,7 @@
         <v>11.11</v>
       </c>
       <c r="D23">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -818,7 +827,7 @@
         <v>11.11</v>
       </c>
       <c r="D24">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -832,7 +841,7 @@
         <v>11.11</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -846,7 +855,7 @@
         <v>11.11</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -860,7 +869,7 @@
         <v>11.11</v>
       </c>
       <c r="D27">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -874,7 +883,7 @@
         <v>11.11</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -888,7 +897,7 @@
         <v>11.11</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -902,7 +911,7 @@
         <v>11.11</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -916,7 +925,7 @@
         <v>11.11</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,7 +939,7 @@
         <v>11.11</v>
       </c>
       <c r="D32">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -944,7 +953,7 @@
         <v>11.11</v>
       </c>
       <c r="D33">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -958,7 +967,7 @@
         <v>11.11</v>
       </c>
       <c r="D34">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -972,7 +981,7 @@
         <v>11.11</v>
       </c>
       <c r="D35">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -986,7 +995,7 @@
         <v>11.11</v>
       </c>
       <c r="D36">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,7 +1009,7 @@
         <v>11.11</v>
       </c>
       <c r="D37">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,7 +1023,7 @@
         <v>11.11</v>
       </c>
       <c r="D38">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,7 +1037,7 @@
         <v>11.11</v>
       </c>
       <c r="D39">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,7 +1051,7 @@
         <v>11.11</v>
       </c>
       <c r="D40">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,7 +1065,7 @@
         <v>11.11</v>
       </c>
       <c r="D41">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,7 +1079,7 @@
         <v>11.11</v>
       </c>
       <c r="D42">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1084,7 +1093,7 @@
         <v>11.11</v>
       </c>
       <c r="D43">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,7 +1107,7 @@
         <v>11.11</v>
       </c>
       <c r="D44">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1112,7 +1121,7 @@
         <v>11.11</v>
       </c>
       <c r="D45">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1126,7 +1135,7 @@
         <v>11.11</v>
       </c>
       <c r="D46">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,7 +1149,7 @@
         <v>11.11</v>
       </c>
       <c r="D47">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,7 +1163,7 @@
         <v>11.11</v>
       </c>
       <c r="D48">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1168,7 +1177,7 @@
         <v>11.11</v>
       </c>
       <c r="D49">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,7 +1191,7 @@
         <v>11.11</v>
       </c>
       <c r="D50">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1196,7 +1205,7 @@
         <v>11.11</v>
       </c>
       <c r="D51">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1210,7 +1219,7 @@
         <v>11.11</v>
       </c>
       <c r="D52">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1224,7 +1233,7 @@
         <v>11.11</v>
       </c>
       <c r="D53">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1238,7 +1247,7 @@
         <v>11.11</v>
       </c>
       <c r="D54">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1252,7 +1261,7 @@
         <v>11.11</v>
       </c>
       <c r="D55">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,7 +1275,7 @@
         <v>11.11</v>
       </c>
       <c r="D56">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1280,7 +1289,7 @@
         <v>11.11</v>
       </c>
       <c r="D57">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,7 +1303,7 @@
         <v>11.11</v>
       </c>
       <c r="D58">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,7 +1317,7 @@
         <v>11.11</v>
       </c>
       <c r="D59">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1322,7 +1331,7 @@
         <v>11.11</v>
       </c>
       <c r="D60">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,7 +1345,7 @@
         <v>11.11</v>
       </c>
       <c r="D61">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1350,7 +1359,7 @@
         <v>12.11</v>
       </c>
       <c r="D62">
-        <v>61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,7 +1373,7 @@
         <v>12.11</v>
       </c>
       <c r="D63">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,7 +1387,7 @@
         <v>12.11</v>
       </c>
       <c r="D64">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,7 +1401,7 @@
         <v>12.11</v>
       </c>
       <c r="D65">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1406,7 +1415,7 @@
         <v>12.11</v>
       </c>
       <c r="D66">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,7 +1429,7 @@
         <v>12.11</v>
       </c>
       <c r="D67">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,7 +1443,7 @@
         <v>12.11</v>
       </c>
       <c r="D68">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,7 +1457,7 @@
         <v>12.11</v>
       </c>
       <c r="D69">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1462,7 +1471,7 @@
         <v>12.11</v>
       </c>
       <c r="D70">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,7 +1485,7 @@
         <v>12.11</v>
       </c>
       <c r="D71">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,7 +1499,7 @@
         <v>13.11</v>
       </c>
       <c r="D72">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1504,7 +1513,7 @@
         <v>13.11</v>
       </c>
       <c r="D73">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1518,7 +1527,7 @@
         <v>13.11</v>
       </c>
       <c r="D74">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1532,7 +1541,7 @@
         <v>13.11</v>
       </c>
       <c r="D75">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1546,7 +1555,7 @@
         <v>13.11</v>
       </c>
       <c r="D76">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1560,7 +1569,7 @@
         <v>13.11</v>
       </c>
       <c r="D77">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1574,7 +1583,7 @@
         <v>13.11</v>
       </c>
       <c r="D78">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1588,7 +1597,7 @@
         <v>13.11</v>
       </c>
       <c r="D79">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1602,7 +1611,7 @@
         <v>13.11</v>
       </c>
       <c r="D80">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1616,7 +1625,7 @@
         <v>13.11</v>
       </c>
       <c r="D81">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1630,7 +1639,7 @@
         <v>13.11</v>
       </c>
       <c r="D82">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1644,7 +1653,7 @@
         <v>13.11</v>
       </c>
       <c r="D83">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1658,7 +1667,7 @@
         <v>13.11</v>
       </c>
       <c r="D84">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1672,7 +1681,7 @@
         <v>13.11</v>
       </c>
       <c r="D85">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1686,7 +1695,7 @@
         <v>13.11</v>
       </c>
       <c r="D86">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1700,7 +1709,7 @@
         <v>13.11</v>
       </c>
       <c r="D87">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1714,7 +1723,7 @@
         <v>13.11</v>
       </c>
       <c r="D88">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -1728,7 +1737,7 @@
         <v>13.11</v>
       </c>
       <c r="D89">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1742,7 +1751,7 @@
         <v>13.11</v>
       </c>
       <c r="D90">
-        <v>89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -1756,7 +1765,7 @@
         <v>13.11</v>
       </c>
       <c r="D91">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -1770,7 +1779,7 @@
         <v>14.11</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -1784,7 +1793,7 @@
         <v>14.11</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -1798,7 +1807,7 @@
         <v>14.11</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -1812,7 +1821,7 @@
         <v>14.11</v>
       </c>
       <c r="D95">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -1826,7 +1835,7 @@
         <v>14.11</v>
       </c>
       <c r="D96">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -1840,7 +1849,7 @@
         <v>14.11</v>
       </c>
       <c r="D97">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -1854,7 +1863,7 @@
         <v>14.11</v>
       </c>
       <c r="D98">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -1868,7 +1877,7 @@
         <v>14.11</v>
       </c>
       <c r="D99">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -1882,7 +1891,7 @@
         <v>14.11</v>
       </c>
       <c r="D100">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -1896,7 +1905,7 @@
         <v>14.11</v>
       </c>
       <c r="D101">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -1910,7 +1919,7 @@
         <v>14.11</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -1924,7 +1933,7 @@
         <v>14.11</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1938,7 +1947,7 @@
         <v>14.11</v>
       </c>
       <c r="D104">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -1952,7 +1961,7 @@
         <v>14.11</v>
       </c>
       <c r="D105">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -1966,7 +1975,7 @@
         <v>14.11</v>
       </c>
       <c r="D106">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -1980,7 +1989,7 @@
         <v>14.11</v>
       </c>
       <c r="D107">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -1994,7 +2003,7 @@
         <v>14.11</v>
       </c>
       <c r="D108">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2008,7 +2017,7 @@
         <v>14.11</v>
       </c>
       <c r="D109">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2022,7 +2031,7 @@
         <v>14.11</v>
       </c>
       <c r="D110">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2036,7 +2045,7 @@
         <v>14.11</v>
       </c>
       <c r="D111">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2050,7 +2059,7 @@
         <v>14.11</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2064,7 +2073,7 @@
         <v>14.11</v>
       </c>
       <c r="D113">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2078,7 +2087,7 @@
         <v>14.11</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2092,7 +2101,7 @@
         <v>14.11</v>
       </c>
       <c r="D115">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2106,7 +2115,7 @@
         <v>14.11</v>
       </c>
       <c r="D116">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2120,7 +2129,7 @@
         <v>14.11</v>
       </c>
       <c r="D117">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2134,7 +2143,7 @@
         <v>14.11</v>
       </c>
       <c r="D118">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2148,7 +2157,7 @@
         <v>14.11</v>
       </c>
       <c r="D119">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2162,7 +2171,7 @@
         <v>14.11</v>
       </c>
       <c r="D120">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2176,7 +2185,7 @@
         <v>14.11</v>
       </c>
       <c r="D121">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2190,7 +2199,7 @@
         <v>14.11</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2204,7 +2213,7 @@
         <v>14.11</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2218,7 +2227,7 @@
         <v>14.11</v>
       </c>
       <c r="D124">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2232,7 +2241,7 @@
         <v>14.11</v>
       </c>
       <c r="D125">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2246,7 +2255,7 @@
         <v>14.11</v>
       </c>
       <c r="D126">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2260,7 +2269,7 @@
         <v>14.11</v>
       </c>
       <c r="D127">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,7 +2283,7 @@
         <v>14.11</v>
       </c>
       <c r="D128">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2288,7 +2297,7 @@
         <v>14.11</v>
       </c>
       <c r="D129">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2302,7 +2311,7 @@
         <v>14.11</v>
       </c>
       <c r="D130">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2316,7 +2325,7 @@
         <v>14.11</v>
       </c>
       <c r="D131">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -2330,7 +2339,7 @@
         <v>14.11</v>
       </c>
       <c r="D132">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2344,7 +2353,7 @@
         <v>14.11</v>
       </c>
       <c r="D133">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2358,7 +2367,7 @@
         <v>14.11</v>
       </c>
       <c r="D134">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2372,7 +2381,7 @@
         <v>14.11</v>
       </c>
       <c r="D135">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -2386,7 +2395,7 @@
         <v>14.11</v>
       </c>
       <c r="D136">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -2400,7 +2409,7 @@
         <v>14.11</v>
       </c>
       <c r="D137">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -2414,7 +2423,7 @@
         <v>14.11</v>
       </c>
       <c r="D138">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -2428,7 +2437,7 @@
         <v>14.11</v>
       </c>
       <c r="D139">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -2442,7 +2451,7 @@
         <v>14.11</v>
       </c>
       <c r="D140">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -2456,7 +2465,7 @@
         <v>14.11</v>
       </c>
       <c r="D141">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -2470,7 +2479,7 @@
         <v>14.11</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -2484,7 +2493,7 @@
         <v>14.11</v>
       </c>
       <c r="D143">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -2498,7 +2507,7 @@
         <v>14.11</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -2512,7 +2521,7 @@
         <v>14.11</v>
       </c>
       <c r="D145">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -2526,7 +2535,7 @@
         <v>14.11</v>
       </c>
       <c r="D146">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -2540,7 +2549,7 @@
         <v>14.11</v>
       </c>
       <c r="D147">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -2554,7 +2563,7 @@
         <v>14.11</v>
       </c>
       <c r="D148">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -2568,7 +2577,7 @@
         <v>14.11</v>
       </c>
       <c r="D149">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -2582,7 +2591,7 @@
         <v>14.11</v>
       </c>
       <c r="D150">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -2596,7 +2605,7 @@
         <v>14.11</v>
       </c>
       <c r="D151">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -2610,7 +2619,7 @@
         <v>14.11</v>
       </c>
       <c r="D152">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -2624,7 +2633,7 @@
         <v>14.11</v>
       </c>
       <c r="D153">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -2638,7 +2647,7 @@
         <v>14.11</v>
       </c>
       <c r="D154">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -2652,7 +2661,7 @@
         <v>14.11</v>
       </c>
       <c r="D155">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -2666,7 +2675,7 @@
         <v>14.11</v>
       </c>
       <c r="D156">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -2680,7 +2689,7 @@
         <v>14.11</v>
       </c>
       <c r="D157">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -2694,7 +2703,7 @@
         <v>14.11</v>
       </c>
       <c r="D158">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -2708,7 +2717,7 @@
         <v>14.11</v>
       </c>
       <c r="D159">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -2722,7 +2731,7 @@
         <v>14.11</v>
       </c>
       <c r="D160">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -2736,7 +2745,7 @@
         <v>14.11</v>
       </c>
       <c r="D161">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -2750,7 +2759,7 @@
         <v>14.11</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -2764,7 +2773,7 @@
         <v>14.11</v>
       </c>
       <c r="D163">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -2778,7 +2787,7 @@
         <v>14.11</v>
       </c>
       <c r="D164">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -2792,7 +2801,7 @@
         <v>14.11</v>
       </c>
       <c r="D165">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -2806,7 +2815,7 @@
         <v>14.11</v>
       </c>
       <c r="D166">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -2820,7 +2829,7 @@
         <v>14.11</v>
       </c>
       <c r="D167">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -2834,7 +2843,7 @@
         <v>14.11</v>
       </c>
       <c r="D168">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -2848,7 +2857,7 @@
         <v>14.11</v>
       </c>
       <c r="D169">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -2862,7 +2871,7 @@
         <v>14.11</v>
       </c>
       <c r="D170">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -2876,7 +2885,7 @@
         <v>14.11</v>
       </c>
       <c r="D171">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -2890,7 +2899,7 @@
         <v>14.11</v>
       </c>
       <c r="D172">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -2904,7 +2913,7 @@
         <v>14.11</v>
       </c>
       <c r="D173">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -2918,7 +2927,7 @@
         <v>14.11</v>
       </c>
       <c r="D174">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -2932,7 +2941,7 @@
         <v>14.11</v>
       </c>
       <c r="D175">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -2946,7 +2955,7 @@
         <v>14.11</v>
       </c>
       <c r="D176">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -2960,7 +2969,7 @@
         <v>14.11</v>
       </c>
       <c r="D177">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -2974,7 +2983,7 @@
         <v>14.11</v>
       </c>
       <c r="D178">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -2988,7 +2997,7 @@
         <v>14.11</v>
       </c>
       <c r="D179">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -3002,7 +3011,7 @@
         <v>14.11</v>
       </c>
       <c r="D180">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -3016,7 +3025,7 @@
         <v>14.11</v>
       </c>
       <c r="D181">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -3030,7 +3039,7 @@
         <v>14.11</v>
       </c>
       <c r="D182">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F182" s="6"/>
     </row>
@@ -3045,7 +3054,7 @@
         <v>14.11</v>
       </c>
       <c r="D183">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F183" s="6"/>
     </row>
@@ -3060,7 +3069,7 @@
         <v>14.11</v>
       </c>
       <c r="D184">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F184" s="6"/>
     </row>
@@ -3075,7 +3084,7 @@
         <v>14.11</v>
       </c>
       <c r="D185">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F185" s="6"/>
     </row>
@@ -3090,7 +3099,7 @@
         <v>14.11</v>
       </c>
       <c r="D186">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F186" s="6"/>
     </row>
@@ -3105,7 +3114,7 @@
         <v>14.11</v>
       </c>
       <c r="D187">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F187" s="6"/>
     </row>
@@ -3120,7 +3129,7 @@
         <v>14.11</v>
       </c>
       <c r="D188">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F188" s="6"/>
     </row>
@@ -3135,7 +3144,7 @@
         <v>14.11</v>
       </c>
       <c r="D189">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F189" s="6"/>
     </row>
@@ -3150,7 +3159,7 @@
         <v>14.11</v>
       </c>
       <c r="D190">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F190" s="6"/>
     </row>
@@ -3165,7 +3174,7 @@
         <v>14.11</v>
       </c>
       <c r="D191">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F191" s="6"/>
     </row>
@@ -3180,7 +3189,7 @@
         <v>14.11</v>
       </c>
       <c r="D192">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F192" s="6"/>
     </row>
@@ -3195,7 +3204,7 @@
         <v>14.11</v>
       </c>
       <c r="D193">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F193" s="6"/>
     </row>
@@ -3210,7 +3219,7 @@
         <v>14.11</v>
       </c>
       <c r="D194">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F194" s="6"/>
     </row>
@@ -3225,7 +3234,7 @@
         <v>14.11</v>
       </c>
       <c r="D195">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F195" s="6"/>
     </row>
@@ -3240,7 +3249,7 @@
         <v>14.11</v>
       </c>
       <c r="D196">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F196" s="6"/>
     </row>
@@ -3255,7 +3264,7 @@
         <v>14.11</v>
       </c>
       <c r="D197">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F197" s="6"/>
     </row>
@@ -3270,7 +3279,7 @@
         <v>14.11</v>
       </c>
       <c r="D198">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F198" s="6"/>
     </row>
@@ -3285,7 +3294,7 @@
         <v>14.11</v>
       </c>
       <c r="D199">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F199" s="6"/>
     </row>
@@ -3300,7 +3309,7 @@
         <v>14.11</v>
       </c>
       <c r="D200">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F200" s="6"/>
     </row>
@@ -3315,7 +3324,7 @@
         <v>14.11</v>
       </c>
       <c r="D201">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F201" s="6"/>
     </row>
@@ -3330,7 +3339,7 @@
         <v>14.11</v>
       </c>
       <c r="D202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F202" s="6"/>
     </row>
@@ -3345,7 +3354,7 @@
         <v>14.11</v>
       </c>
       <c r="D203">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F203" s="6"/>
     </row>
@@ -3360,7 +3369,7 @@
         <v>14.11</v>
       </c>
       <c r="D204">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F204" s="6"/>
     </row>
@@ -3375,7 +3384,7 @@
         <v>14.11</v>
       </c>
       <c r="D205">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F205" s="6"/>
     </row>
@@ -3390,7 +3399,7 @@
         <v>14.11</v>
       </c>
       <c r="D206">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F206" s="6"/>
     </row>
@@ -3405,7 +3414,7 @@
         <v>14.11</v>
       </c>
       <c r="D207">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F207" s="6"/>
     </row>
@@ -3420,7 +3429,7 @@
         <v>14.11</v>
       </c>
       <c r="D208">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F208" s="6"/>
     </row>
@@ -3435,7 +3444,7 @@
         <v>14.11</v>
       </c>
       <c r="D209">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F209" s="6"/>
     </row>
@@ -3450,7 +3459,7 @@
         <v>14.11</v>
       </c>
       <c r="D210">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F210" s="6"/>
     </row>
@@ -3465,7 +3474,7 @@
         <v>14.11</v>
       </c>
       <c r="D211">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F211" s="6"/>
     </row>
@@ -3480,7 +3489,7 @@
         <v>14.11</v>
       </c>
       <c r="D212">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F212" s="6"/>
     </row>
@@ -3495,7 +3504,7 @@
         <v>14.11</v>
       </c>
       <c r="D213">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F213" s="6"/>
     </row>
@@ -3510,7 +3519,7 @@
         <v>14.11</v>
       </c>
       <c r="D214">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F214" s="6"/>
     </row>
@@ -3525,7 +3534,7 @@
         <v>14.11</v>
       </c>
       <c r="D215">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F215" s="6"/>
     </row>
@@ -3540,7 +3549,7 @@
         <v>14.11</v>
       </c>
       <c r="D216">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F216" s="6"/>
     </row>
@@ -3555,7 +3564,7 @@
         <v>14.11</v>
       </c>
       <c r="D217">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F217" s="6"/>
     </row>
@@ -3570,7 +3579,7 @@
         <v>14.11</v>
       </c>
       <c r="D218">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F218" s="6"/>
     </row>
@@ -3585,7 +3594,7 @@
         <v>14.11</v>
       </c>
       <c r="D219">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F219" s="6"/>
     </row>
@@ -3600,7 +3609,7 @@
         <v>14.11</v>
       </c>
       <c r="D220">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F220" s="6"/>
     </row>
@@ -3615,9 +3624,1087 @@
         <v>14.11</v>
       </c>
       <c r="D221">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F221" s="6"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="6">
+        <v>1028671</v>
+      </c>
+      <c r="B222">
+        <v>0</v>
+      </c>
+      <c r="C222">
+        <v>15.11</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="6">
+        <v>2298689</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <v>15.11</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="6">
+        <v>7521477</v>
+      </c>
+      <c r="B224">
+        <v>-1</v>
+      </c>
+      <c r="C224">
+        <v>15.11</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="6">
+        <v>34319106</v>
+      </c>
+      <c r="B225">
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <v>15.11</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="6">
+        <v>28388755</v>
+      </c>
+      <c r="B226">
+        <v>-1</v>
+      </c>
+      <c r="C226">
+        <v>15.11</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="6">
+        <v>24048171</v>
+      </c>
+      <c r="B227">
+        <v>-1</v>
+      </c>
+      <c r="C227">
+        <v>15.11</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="6">
+        <v>20138604</v>
+      </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <v>15.11</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="6">
+        <v>24292756</v>
+      </c>
+      <c r="B229">
+        <v>1</v>
+      </c>
+      <c r="C229">
+        <v>15.11</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="6">
+        <v>17839776</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <v>15.11</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="6">
+        <v>12095072</v>
+      </c>
+      <c r="B231">
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <v>15.11</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="6">
+        <v>24021186</v>
+      </c>
+      <c r="B232">
+        <v>-1</v>
+      </c>
+      <c r="C232">
+        <v>15.11</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="6">
+        <v>30975925</v>
+      </c>
+      <c r="B233">
+        <v>1</v>
+      </c>
+      <c r="C233">
+        <v>15.11</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="6">
+        <v>3389311</v>
+      </c>
+      <c r="B234">
+        <v>1</v>
+      </c>
+      <c r="C234">
+        <v>15.11</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="6">
+        <v>4600837</v>
+      </c>
+      <c r="B235">
+        <v>1</v>
+      </c>
+      <c r="C235">
+        <v>15.11</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="6">
+        <v>5137345</v>
+      </c>
+      <c r="B236">
+        <v>1</v>
+      </c>
+      <c r="C236">
+        <v>15.11</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="6">
+        <v>14613957</v>
+      </c>
+      <c r="B237">
+        <v>1</v>
+      </c>
+      <c r="C237">
+        <v>15.11</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="6">
+        <v>24665535</v>
+      </c>
+      <c r="B238">
+        <v>1</v>
+      </c>
+      <c r="C238">
+        <v>15.11</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="6">
+        <v>2397783</v>
+      </c>
+      <c r="B239">
+        <v>0</v>
+      </c>
+      <c r="C239">
+        <v>15.11</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="6">
+        <v>1472852</v>
+      </c>
+      <c r="B240">
+        <v>-1</v>
+      </c>
+      <c r="C240">
+        <v>15.11</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="6">
+        <v>31032524</v>
+      </c>
+      <c r="B241">
+        <v>1</v>
+      </c>
+      <c r="C241">
+        <v>15.11</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="6">
+        <v>4644031</v>
+      </c>
+      <c r="B242">
+        <v>0</v>
+      </c>
+      <c r="C242">
+        <v>15.11</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="6">
+        <v>19152358</v>
+      </c>
+      <c r="B243">
+        <v>1</v>
+      </c>
+      <c r="C243">
+        <v>15.11</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="6">
+        <v>25411775</v>
+      </c>
+      <c r="B244">
+        <v>0</v>
+      </c>
+      <c r="C244">
+        <v>15.11</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="6">
+        <v>15706563</v>
+      </c>
+      <c r="B245">
+        <v>0</v>
+      </c>
+      <c r="C245">
+        <v>15.11</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="6">
+        <v>15036863</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <v>15.11</v>
+      </c>
+      <c r="D246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="6">
+        <v>12048544</v>
+      </c>
+      <c r="B247">
+        <v>1</v>
+      </c>
+      <c r="C247">
+        <v>15.11</v>
+      </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="6">
+        <v>12138493</v>
+      </c>
+      <c r="B248">
+        <v>-1</v>
+      </c>
+      <c r="C248">
+        <v>15.11</v>
+      </c>
+      <c r="D248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="6">
+        <v>14168925</v>
+      </c>
+      <c r="B249">
+        <v>1</v>
+      </c>
+      <c r="C249">
+        <v>15.11</v>
+      </c>
+      <c r="D249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" s="6">
+        <v>15397835</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250">
+        <v>15.11</v>
+      </c>
+      <c r="D250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="6">
+        <v>36353797</v>
+      </c>
+      <c r="B251">
+        <v>1</v>
+      </c>
+      <c r="C251">
+        <v>15.11</v>
+      </c>
+      <c r="D251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="6">
+        <v>4278437</v>
+      </c>
+      <c r="B252">
+        <v>-1</v>
+      </c>
+      <c r="C252">
+        <v>15.11</v>
+      </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="6">
+        <v>6691690</v>
+      </c>
+      <c r="B253">
+        <v>1</v>
+      </c>
+      <c r="C253">
+        <v>15.11</v>
+      </c>
+      <c r="D253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="6">
+        <v>26057620</v>
+      </c>
+      <c r="B254">
+        <v>0</v>
+      </c>
+      <c r="C254">
+        <v>15.11</v>
+      </c>
+      <c r="D254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="6">
+        <v>19278375</v>
+      </c>
+      <c r="B255">
+        <v>-1</v>
+      </c>
+      <c r="C255">
+        <v>15.11</v>
+      </c>
+      <c r="D255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="6">
+        <v>4907371</v>
+      </c>
+      <c r="B256">
+        <v>0</v>
+      </c>
+      <c r="C256">
+        <v>15.11</v>
+      </c>
+      <c r="D256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="6">
+        <v>25105934</v>
+      </c>
+      <c r="B257">
+        <v>-1</v>
+      </c>
+      <c r="C257">
+        <v>15.11</v>
+      </c>
+      <c r="D257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="6">
+        <v>113454</v>
+      </c>
+      <c r="B258">
+        <v>-1</v>
+      </c>
+      <c r="C258">
+        <v>15.11</v>
+      </c>
+      <c r="D258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="6">
+        <v>19046062</v>
+      </c>
+      <c r="B259">
+        <v>0</v>
+      </c>
+      <c r="C259">
+        <v>15.11</v>
+      </c>
+      <c r="D259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="6">
+        <v>24954740</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+      <c r="C260">
+        <v>15.11</v>
+      </c>
+      <c r="D260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="6">
+        <v>18967674</v>
+      </c>
+      <c r="B261">
+        <v>-1</v>
+      </c>
+      <c r="C261">
+        <v>15.11</v>
+      </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="6">
+        <v>76413571</v>
+      </c>
+      <c r="B262">
+        <v>0</v>
+      </c>
+      <c r="C262">
+        <v>15.11</v>
+      </c>
+      <c r="D262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="6">
+        <v>13201569</v>
+      </c>
+      <c r="B263">
+        <v>0</v>
+      </c>
+      <c r="C263">
+        <v>15.11</v>
+      </c>
+      <c r="D263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="6">
+        <v>24214688</v>
+      </c>
+      <c r="B264">
+        <v>-1</v>
+      </c>
+      <c r="C264">
+        <v>15.11</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="6">
+        <v>30199617</v>
+      </c>
+      <c r="B265">
+        <v>-1</v>
+      </c>
+      <c r="C265">
+        <v>15.11</v>
+      </c>
+      <c r="D265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="6">
+        <v>1336564</v>
+      </c>
+      <c r="B266">
+        <v>0</v>
+      </c>
+      <c r="C266">
+        <v>15.11</v>
+      </c>
+      <c r="D266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="6">
+        <v>34573784</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+      <c r="C267">
+        <v>15.11</v>
+      </c>
+      <c r="D267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" s="6">
+        <v>5289480</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+      <c r="C268">
+        <v>15.11</v>
+      </c>
+      <c r="D268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" s="6">
+        <v>23664512</v>
+      </c>
+      <c r="B269">
+        <v>0</v>
+      </c>
+      <c r="C269">
+        <v>15.11</v>
+      </c>
+      <c r="D269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" s="6">
+        <v>19301429</v>
+      </c>
+      <c r="B270">
+        <v>-1</v>
+      </c>
+      <c r="C270">
+        <v>15.11</v>
+      </c>
+      <c r="D270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" s="6">
+        <v>8777711</v>
+      </c>
+      <c r="B271">
+        <v>1</v>
+      </c>
+      <c r="C271">
+        <v>15.11</v>
+      </c>
+      <c r="D271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" s="7">
+        <v>14060163</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+      <c r="C272">
+        <v>15.11</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" s="7">
+        <v>14144257</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273">
+        <v>15.11</v>
+      </c>
+      <c r="D273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" s="7">
+        <v>21787356</v>
+      </c>
+      <c r="B274">
+        <v>0</v>
+      </c>
+      <c r="C274">
+        <v>15.11</v>
+      </c>
+      <c r="D274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" s="7">
+        <v>24104622</v>
+      </c>
+      <c r="B275">
+        <v>0</v>
+      </c>
+      <c r="C275">
+        <v>15.11</v>
+      </c>
+      <c r="D275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" s="7">
+        <v>25874731</v>
+      </c>
+      <c r="B276">
+        <v>0</v>
+      </c>
+      <c r="C276">
+        <v>15.11</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="7">
+        <v>29651684</v>
+      </c>
+      <c r="B277">
+        <v>1</v>
+      </c>
+      <c r="C277">
+        <v>15.11</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="7">
+        <v>16994537</v>
+      </c>
+      <c r="B278">
+        <v>0</v>
+      </c>
+      <c r="C278">
+        <v>15.11</v>
+      </c>
+      <c r="D278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="7">
+        <v>18950355</v>
+      </c>
+      <c r="B279">
+        <v>1</v>
+      </c>
+      <c r="C279">
+        <v>15.11</v>
+      </c>
+      <c r="D279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="7">
+        <v>19389678</v>
+      </c>
+      <c r="B280">
+        <v>-1</v>
+      </c>
+      <c r="C280">
+        <v>15.11</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="7">
+        <v>21472296</v>
+      </c>
+      <c r="B281">
+        <v>0</v>
+      </c>
+      <c r="C281">
+        <v>15.11</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="7">
+        <v>24631652</v>
+      </c>
+      <c r="B282">
+        <v>-1</v>
+      </c>
+      <c r="C282">
+        <v>15.11</v>
+      </c>
+      <c r="D282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="7">
+        <v>24815671</v>
+      </c>
+      <c r="B283">
+        <v>-1</v>
+      </c>
+      <c r="C283">
+        <v>15.11</v>
+      </c>
+      <c r="D283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284" s="7">
+        <v>26016562</v>
+      </c>
+      <c r="B284">
+        <v>0</v>
+      </c>
+      <c r="C284">
+        <v>15.11</v>
+      </c>
+      <c r="D284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" s="7">
+        <v>27286055</v>
+      </c>
+      <c r="B285">
+        <v>0</v>
+      </c>
+      <c r="C285">
+        <v>15.11</v>
+      </c>
+      <c r="D285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="7">
+        <v>28852030</v>
+      </c>
+      <c r="B286">
+        <v>-1</v>
+      </c>
+      <c r="C286">
+        <v>15.11</v>
+      </c>
+      <c r="D286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" s="7">
+        <v>28932258</v>
+      </c>
+      <c r="B287">
+        <v>0</v>
+      </c>
+      <c r="C287">
+        <v>15.11</v>
+      </c>
+      <c r="D287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="7">
+        <v>29499560</v>
+      </c>
+      <c r="B288">
+        <v>1</v>
+      </c>
+      <c r="C288">
+        <v>15.11</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A289" s="7">
+        <v>2154704</v>
+      </c>
+      <c r="B289">
+        <v>0</v>
+      </c>
+      <c r="C289">
+        <v>15.11</v>
+      </c>
+      <c r="D289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A290" s="7">
+        <v>3477618</v>
+      </c>
+      <c r="B290">
+        <v>0</v>
+      </c>
+      <c r="C290">
+        <v>15.11</v>
+      </c>
+      <c r="D290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A291" s="7">
+        <v>3597370</v>
+      </c>
+      <c r="B291">
+        <v>1</v>
+      </c>
+      <c r="C291">
+        <v>15.11</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A292" s="7">
+        <v>3883051</v>
+      </c>
+      <c r="B292">
+        <v>1</v>
+      </c>
+      <c r="C292">
+        <v>15.11</v>
+      </c>
+      <c r="D292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A293" s="7">
+        <v>6714641</v>
+      </c>
+      <c r="B293">
+        <v>1</v>
+      </c>
+      <c r="C293">
+        <v>15.11</v>
+      </c>
+      <c r="D293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A294" s="7">
+        <v>8411320</v>
+      </c>
+      <c r="B294">
+        <v>-1</v>
+      </c>
+      <c r="C294">
+        <v>15.11</v>
+      </c>
+      <c r="D294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A295" s="7">
+        <v>18950355</v>
+      </c>
+      <c r="B295">
+        <v>1</v>
+      </c>
+      <c r="C295">
+        <v>15.11</v>
+      </c>
+      <c r="D295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A296" s="7">
+        <v>19389678</v>
+      </c>
+      <c r="B296">
+        <v>-1</v>
+      </c>
+      <c r="C296">
+        <v>15.11</v>
+      </c>
+      <c r="D296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A297" s="7">
+        <v>24815671</v>
+      </c>
+      <c r="B297">
+        <v>-1</v>
+      </c>
+      <c r="C297">
+        <v>15.11</v>
+      </c>
+      <c r="D297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298" s="7">
+        <v>28932258</v>
+      </c>
+      <c r="B298">
+        <v>-1</v>
+      </c>
+      <c r="C298">
+        <v>15.11</v>
+      </c>
+      <c r="D298">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B103 B222:B1048576">
@@ -3647,6 +4734,194 @@
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B121 B222:B1048576">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94:B121 B222:B229">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122:B161">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B162:B181">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B164:B181">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B182:B221">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3680,8 +4955,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:B121 B222:B229">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="G182:G222">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="4" tint="0.79998168889431442"/>
+        <color theme="6" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3691,30 +4986,6 @@
         <color theme="9" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B121 B222:B1048576">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G182:G222">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3744,202 +5015,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G182:G222">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="9" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G182:G222">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B122:B161">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B122:B161">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="9" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B122:B161">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B164:B181">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B162:B181">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="9" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B162:B181">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B182:B221">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="9" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B182:B221">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="4" tint="0.79998168889431442"/>
-        <color theme="6" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
oups a mislabelled point, fixed
</commit_message>
<xml_diff>
--- a/data/RAW/Human_labelling_violentMovie.xlsx
+++ b/data/RAW/Human_labelling_violentMovie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djay/Desktop/ADA/ada-2024-project-alligatorsdontapologize24/data/RAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E9EC7-370F-F84C-8242-F37883193F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A567F-2D29-EB4A-96CC-B42501BCA63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15740" windowHeight="17440" xr2:uid="{39CBA11C-2844-B64A-9A4E-B9281B3D6EC7}"/>
   </bookViews>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B92C561-11BB-6946-9D59-BAB10DC0BC04}">
-  <dimension ref="A1:F298"/>
+  <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="B299" sqref="B299"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="6">
-        <v>76413571</v>
+        <v>13201569</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="6">
-        <v>13201569</v>
+        <v>24214688</v>
       </c>
       <c r="B263">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C263">
         <v>15.11</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="6">
-        <v>24214688</v>
+        <v>30199617</v>
       </c>
       <c r="B264">
         <v>-1</v>
@@ -4232,10 +4232,10 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="6">
-        <v>30199617</v>
+        <v>1336564</v>
       </c>
       <c r="B265">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C265">
         <v>15.11</v>
@@ -4246,10 +4246,10 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="6">
-        <v>1336564</v>
+        <v>34573784</v>
       </c>
       <c r="B266">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C266">
         <v>15.11</v>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="6">
-        <v>34573784</v>
+        <v>5289480</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -4274,10 +4274,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="6">
-        <v>5289480</v>
+        <v>23664512</v>
       </c>
       <c r="B268">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C268">
         <v>15.11</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="6">
-        <v>23664512</v>
+        <v>19301429</v>
       </c>
       <c r="B269">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C269">
         <v>15.11</v>
@@ -4302,10 +4302,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="6">
-        <v>19301429</v>
+        <v>8777711</v>
       </c>
       <c r="B270">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C270">
         <v>15.11</v>
@@ -4315,8 +4315,8 @@
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A271" s="6">
-        <v>8777711</v>
+      <c r="A271" s="7">
+        <v>14060163</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -4325,12 +4325,12 @@
         <v>15.11</v>
       </c>
       <c r="D271">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="7">
-        <v>14060163</v>
+        <v>14144257</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -4344,10 +4344,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="7">
-        <v>14144257</v>
+        <v>21787356</v>
       </c>
       <c r="B273">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C273">
         <v>15.11</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="7">
-        <v>21787356</v>
+        <v>24104622</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -4372,7 +4372,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="7">
-        <v>24104622</v>
+        <v>25874731</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="7">
-        <v>25874731</v>
+        <v>29651684</v>
       </c>
       <c r="B276">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C276">
         <v>15.11</v>
@@ -4400,10 +4400,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="7">
-        <v>29651684</v>
+        <v>16994537</v>
       </c>
       <c r="B277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C277">
         <v>15.11</v>
@@ -4414,10 +4414,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="7">
-        <v>16994537</v>
+        <v>18950355</v>
       </c>
       <c r="B278">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C278">
         <v>15.11</v>
@@ -4428,10 +4428,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="7">
-        <v>18950355</v>
+        <v>19389678</v>
       </c>
       <c r="B279">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C279">
         <v>15.11</v>
@@ -4442,10 +4442,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="7">
-        <v>19389678</v>
+        <v>21472296</v>
       </c>
       <c r="B280">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C280">
         <v>15.11</v>
@@ -4456,10 +4456,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="7">
-        <v>21472296</v>
+        <v>24631652</v>
       </c>
       <c r="B281">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C281">
         <v>15.11</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="7">
-        <v>24631652</v>
+        <v>24815671</v>
       </c>
       <c r="B282">
         <v>-1</v>
@@ -4484,10 +4484,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="7">
-        <v>24815671</v>
+        <v>26016562</v>
       </c>
       <c r="B283">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C283">
         <v>15.11</v>
@@ -4498,7 +4498,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="7">
-        <v>26016562</v>
+        <v>27286055</v>
       </c>
       <c r="B284">
         <v>0</v>
@@ -4512,10 +4512,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="7">
-        <v>27286055</v>
+        <v>28852030</v>
       </c>
       <c r="B285">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C285">
         <v>15.11</v>
@@ -4526,10 +4526,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="7">
-        <v>28852030</v>
+        <v>28932258</v>
       </c>
       <c r="B286">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C286">
         <v>15.11</v>
@@ -4540,10 +4540,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="7">
-        <v>28932258</v>
+        <v>29499560</v>
       </c>
       <c r="B287">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C287">
         <v>15.11</v>
@@ -4554,10 +4554,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="7">
-        <v>29499560</v>
+        <v>2154704</v>
       </c>
       <c r="B288">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C288">
         <v>15.11</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="7">
-        <v>2154704</v>
+        <v>3477618</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -4582,10 +4582,10 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="7">
-        <v>3477618</v>
+        <v>3597370</v>
       </c>
       <c r="B290">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C290">
         <v>15.11</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="7">
-        <v>3597370</v>
+        <v>3883051</v>
       </c>
       <c r="B291">
         <v>1</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="7">
-        <v>3883051</v>
+        <v>6714641</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -4624,10 +4624,10 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="7">
-        <v>6714641</v>
+        <v>8411320</v>
       </c>
       <c r="B293">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C293">
         <v>15.11</v>
@@ -4638,10 +4638,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
-        <v>8411320</v>
+        <v>18950355</v>
       </c>
       <c r="B294">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C294">
         <v>15.11</v>
@@ -4652,10 +4652,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="7">
-        <v>18950355</v>
+        <v>19389678</v>
       </c>
       <c r="B295">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C295">
         <v>15.11</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="7">
-        <v>19389678</v>
+        <v>24815671</v>
       </c>
       <c r="B296">
         <v>-1</v>
@@ -4680,7 +4680,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="7">
-        <v>24815671</v>
+        <v>28932258</v>
       </c>
       <c r="B297">
         <v>-1</v>
@@ -4689,20 +4689,6 @@
         <v>15.11</v>
       </c>
       <c r="D297">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A298" s="7">
-        <v>28932258</v>
-      </c>
-      <c r="B298">
-        <v>-1</v>
-      </c>
-      <c r="C298">
-        <v>15.11</v>
-      </c>
-      <c r="D298">
         <v>1</v>
       </c>
     </row>

</xml_diff>